<commit_message>
actualizo archivos de bbdd
</commit_message>
<xml_diff>
--- a/Documentacion/Diccionario de datos.xlsx
+++ b/Documentacion/Diccionario de datos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="225">
   <si>
     <t>Tabla</t>
   </si>
@@ -607,6 +607,93 @@
   </si>
   <si>
     <t>id_customer</t>
+  </si>
+  <si>
+    <t>Triggers de la Tabla</t>
+  </si>
+  <si>
+    <t>precio_compra</t>
+  </si>
+  <si>
+    <t>Setea el precio de la compra según los precios de cada item</t>
+  </si>
+  <si>
+    <t>check_state_purch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chequea cambios de estado de la compra </t>
+  </si>
+  <si>
+    <t>update_stock_purch</t>
+  </si>
+  <si>
+    <t>Resta o suma stock cuando cambia el estado de la compra</t>
+  </si>
+  <si>
+    <t>check_purch</t>
+  </si>
+  <si>
+    <t>evitar updates y deletes de una compra (cuando está cancelada, pendiente o completada)</t>
+  </si>
+  <si>
+    <t>update_stock</t>
+  </si>
+  <si>
+    <t>Reestablece stock cuando vence la reserva</t>
+  </si>
+  <si>
+    <t>check_state_res</t>
+  </si>
+  <si>
+    <t>Chequea cambios de estado de la reserva</t>
+  </si>
+  <si>
+    <t>Evita updates y deletes de una reserva activa</t>
+  </si>
+  <si>
+    <t>check_res</t>
+  </si>
+  <si>
+    <t>check_coupon_date</t>
+  </si>
+  <si>
+    <t>Chequea que la fecha de vencimiento del cupón no sea anterior a la actual</t>
+  </si>
+  <si>
+    <t>check_ship</t>
+  </si>
+  <si>
+    <t>Evita updates de la informacion del envio - excepto el track_code</t>
+  </si>
+  <si>
+    <t>date_msg</t>
+  </si>
+  <si>
+    <t>Setea fecha actual al cargarse el mensaje</t>
+  </si>
+  <si>
+    <t>date_purch</t>
+  </si>
+  <si>
+    <t>Setea fecha acutal al cargar o actualizar compra</t>
+  </si>
+  <si>
+    <t>date_res</t>
+  </si>
+  <si>
+    <t>Setea fecha actual al cargar la reserva</t>
+  </si>
+  <si>
+    <t>date_wsh</t>
+  </si>
+  <si>
+    <t>Setea fecha actual al cargar un producto a la lista de deseados</t>
+  </si>
+  <si>
+    <t>date_rev</t>
+  </si>
+  <si>
+    <t>Setea fecha actual al cargar o actualizar una review</t>
   </si>
 </sst>
 </file>
@@ -1047,9 +1134,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:H131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G127" sqref="G127"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1058,7 +1147,8 @@
     <col min="3" max="3" width="25.77734375" customWidth="1"/>
     <col min="4" max="5" width="13.6640625" customWidth="1"/>
     <col min="6" max="6" width="38.5546875" customWidth="1"/>
-    <col min="7" max="7" width="30.21875" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
+    <col min="8" max="8" width="74.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1216,7 +1306,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>0</v>
       </c>
@@ -1235,8 +1325,14 @@
       <c r="F17" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>2</v>
       </c>
@@ -1255,8 +1351,10 @@
       <c r="F18" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6" t="s">
         <v>110</v>
@@ -1273,9 +1371,11 @@
       <c r="F19" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>0</v>
       </c>
@@ -1294,8 +1394,14 @@
       <c r="F22" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
         <v>10</v>
       </c>
@@ -1314,8 +1420,10 @@
       <c r="F23" s="13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>110</v>
@@ -1332,8 +1440,10 @@
       <c r="F24" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12" t="s">
@@ -1348,8 +1458,10 @@
       <c r="F25" s="12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>154</v>
@@ -1366,9 +1478,11 @@
       <c r="F26" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
         <v>0</v>
       </c>
@@ -1387,8 +1501,14 @@
       <c r="F28" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>23</v>
       </c>
@@ -1407,8 +1527,10 @@
       <c r="F29" s="13" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
@@ -1423,8 +1545,10 @@
       <c r="F30" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6" t="s">
@@ -1439,8 +1563,10 @@
       <c r="F31" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
@@ -1455,8 +1581,10 @@
       <c r="F32" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6" t="s">
@@ -1471,8 +1599,10 @@
       <c r="F33" s="6" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
@@ -1487,8 +1617,10 @@
       <c r="F34" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6" t="s">
@@ -1503,8 +1635,10 @@
       <c r="F35" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
@@ -1519,8 +1653,10 @@
       <c r="F36" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
       <c r="B37" s="6" t="s">
         <v>155</v>
@@ -1537,9 +1673,11 @@
       <c r="F37" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="8" t="s">
         <v>0</v>
       </c>
@@ -1558,8 +1696,14 @@
       <c r="F39" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>40</v>
       </c>
@@ -1578,8 +1722,10 @@
       <c r="F40" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
       <c r="B41" s="6" t="s">
         <v>156</v>
@@ -1596,8 +1742,10 @@
       <c r="F41" s="6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
         <v>157</v>
@@ -1614,12 +1762,14 @@
       <c r="F42" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B43" s="5"/>
     </row>
-    <row r="44" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="45" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="8" t="s">
         <v>0</v>
       </c>
@@ -1638,8 +1788,14 @@
       <c r="F45" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G45" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>51</v>
       </c>
@@ -1658,8 +1814,14 @@
       <c r="F46" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G46" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
       <c r="B47" s="6" t="s">
         <v>56</v>
@@ -1676,8 +1838,10 @@
       <c r="F47" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
@@ -1692,8 +1856,10 @@
       <c r="F48" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
       <c r="B49" s="6" t="s">
         <v>149</v>
@@ -1710,8 +1876,10 @@
       <c r="F49" s="6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
         <v>158</v>
@@ -1728,9 +1896,11 @@
       <c r="F50" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="53" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+    </row>
+    <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="8" t="s">
         <v>0</v>
       </c>
@@ -1749,8 +1919,14 @@
       <c r="F53" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G53" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H53" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>57</v>
       </c>
@@ -1769,8 +1945,10 @@
       <c r="F54" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6" t="s">
@@ -1785,9 +1963,11 @@
       <c r="F55" s="6" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="58" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+    </row>
+    <row r="57" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="58" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="8" t="s">
         <v>0</v>
       </c>
@@ -1806,8 +1986,14 @@
       <c r="F58" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G58" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>66</v>
       </c>
@@ -1826,8 +2012,10 @@
       <c r="F59" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
       <c r="B60" s="6" t="s">
         <v>56</v>
@@ -1844,8 +2032,10 @@
       <c r="F60" s="6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
         <v>162</v>
@@ -1862,8 +2052,10 @@
       <c r="F61" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="6"/>
       <c r="B62" s="6" t="s">
         <v>56</v>
@@ -1880,8 +2072,10 @@
       <c r="F62" s="6" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1" t="s">
         <v>56</v>
@@ -1898,8 +2092,10 @@
       <c r="F63" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="6"/>
       <c r="B64" s="6" t="s">
         <v>56</v>
@@ -1916,8 +2112,10 @@
       <c r="F64" s="6" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1" t="s">
         <v>159</v>
@@ -1934,8 +2132,10 @@
       <c r="F65" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="6"/>
       <c r="B66" s="6" t="s">
         <v>163</v>
@@ -1952,8 +2152,10 @@
       <c r="F66" s="6" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1" t="s">
         <v>56</v>
@@ -1970,10 +2172,12 @@
       <c r="F67" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="70" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+    </row>
+    <row r="68" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="70" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="8" t="s">
         <v>0</v>
       </c>
@@ -1992,8 +2196,14 @@
       <c r="F70" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G70" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H70" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>83</v>
       </c>
@@ -2012,8 +2222,10 @@
       <c r="F71" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6" t="s">
@@ -2028,8 +2240,10 @@
       <c r="F72" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
@@ -2044,8 +2258,10 @@
       <c r="F73" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="6"/>
       <c r="B74" s="6" t="s">
         <v>163</v>
@@ -2062,8 +2278,10 @@
       <c r="F74" s="6" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1" t="s">
         <v>153</v>
@@ -2080,9 +2298,11 @@
       <c r="F75" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="78" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+    </row>
+    <row r="77" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="78" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="8" t="s">
         <v>0</v>
       </c>
@@ -2101,8 +2321,14 @@
       <c r="F78" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G78" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H78" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>94</v>
       </c>
@@ -2121,8 +2347,14 @@
       <c r="F79" s="3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G79" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="H79" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6" t="s">
@@ -2137,8 +2369,10 @@
       <c r="F80" s="6" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1" t="s">
@@ -2153,9 +2387,11 @@
       <c r="F81" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="84" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+    </row>
+    <row r="83" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="84" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="8" t="s">
         <v>0</v>
       </c>
@@ -2174,8 +2410,14 @@
       <c r="F84" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G84" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H84" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>100</v>
       </c>
@@ -2194,8 +2436,14 @@
       <c r="F85" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G85" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6" t="s">
@@ -2210,8 +2458,10 @@
       <c r="F86" s="6" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1" t="s">
@@ -2226,8 +2476,10 @@
       <c r="F87" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6" t="s">
@@ -2242,8 +2494,10 @@
       <c r="F88" s="6" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1" t="s">
@@ -2258,8 +2512,10 @@
       <c r="F89" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6" t="s">
@@ -2274,8 +2530,10 @@
       <c r="F90" s="6" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="1" t="s">
         <v>110</v>
@@ -2292,8 +2550,10 @@
       <c r="F91" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6" t="s">
@@ -2308,9 +2568,11 @@
       <c r="F92" s="6" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="95" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
+    </row>
+    <row r="94" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="95" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="8" t="s">
         <v>0</v>
       </c>
@@ -2329,8 +2591,14 @@
       <c r="F95" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G95" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H95" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>113</v>
       </c>
@@ -2349,10 +2617,18 @@
       <c r="F96" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G96" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="6"/>
-      <c r="B97" s="6"/>
+      <c r="B97" s="6" t="s">
+        <v>163</v>
+      </c>
       <c r="C97" s="6" t="s">
         <v>71</v>
       </c>
@@ -2365,8 +2641,14 @@
       <c r="F97" s="6" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G97" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="H97" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1" t="s">
@@ -2381,8 +2663,14 @@
       <c r="F98" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G98" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="6"/>
       <c r="B99" s="6"/>
       <c r="C99" s="6" t="s">
@@ -2397,8 +2685,14 @@
       <c r="F99" s="6" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G99" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H99" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="1"/>
       <c r="B100" s="1" t="s">
         <v>149</v>
@@ -2415,8 +2709,14 @@
       <c r="F100" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G100" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="6"/>
       <c r="B101" s="6" t="s">
         <v>160</v>
@@ -2433,8 +2733,10 @@
       <c r="F101" s="6" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="1"/>
       <c r="B102" s="1" t="s">
         <v>161</v>
@@ -2451,9 +2753,11 @@
       <c r="F102" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="105" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+    </row>
+    <row r="104" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="105" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="8" t="s">
         <v>0</v>
       </c>
@@ -2472,8 +2776,14 @@
       <c r="F105" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G105" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H105" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>123</v>
       </c>
@@ -2492,8 +2802,10 @@
       <c r="F106" s="3" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G106" s="3"/>
+      <c r="H106" s="3"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="6"/>
       <c r="B107" s="6" t="s">
         <v>19</v>
@@ -2510,8 +2822,10 @@
       <c r="F107" s="6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G107" s="6"/>
+      <c r="H107" s="6"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1" t="s">
@@ -2526,9 +2840,11 @@
       <c r="F108" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="110" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+    </row>
+    <row r="109" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="110" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="8" t="s">
         <v>0</v>
       </c>
@@ -2547,8 +2863,14 @@
       <c r="F110" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G110" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H110" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>127</v>
       </c>
@@ -2567,8 +2889,14 @@
       <c r="F111" s="3" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G111" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="H111" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="6"/>
       <c r="B112" s="6"/>
       <c r="C112" s="6" t="s">
@@ -2583,8 +2911,14 @@
       <c r="F112" s="6" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G112" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="H112" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1" t="s">
@@ -2599,8 +2933,14 @@
       <c r="F113" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G113" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="6"/>
       <c r="B114" s="6" t="s">
         <v>149</v>
@@ -2617,8 +2957,14 @@
       <c r="F114" s="6" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G114" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="H114" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="1"/>
       <c r="B115" s="1" t="s">
         <v>150</v>
@@ -2635,8 +2981,10 @@
       <c r="F115" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G115" s="1"/>
+      <c r="H115" s="1"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="6"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6" t="s">
@@ -2651,9 +2999,11 @@
       <c r="F116" s="6" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="119" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G116" s="6"/>
+      <c r="H116" s="6"/>
+    </row>
+    <row r="118" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="119" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="8" t="s">
         <v>0</v>
       </c>
@@ -2672,8 +3022,14 @@
       <c r="F119" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G119" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H119" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
         <v>133</v>
       </c>
@@ -2692,8 +3048,14 @@
       <c r="F120" s="3" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G120" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="H120" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="6"/>
       <c r="B121" s="6" t="s">
         <v>152</v>
@@ -2710,8 +3072,10 @@
       <c r="F121" s="6" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G121" s="6"/>
+      <c r="H121" s="6"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1" t="s">
@@ -2726,9 +3090,11 @@
       <c r="F122" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="125" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G122" s="1"/>
+      <c r="H122" s="1"/>
+    </row>
+    <row r="124" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="125" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="8" t="s">
         <v>0</v>
       </c>
@@ -2747,8 +3113,14 @@
       <c r="F125" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G125" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H125" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
         <v>137</v>
       </c>
@@ -2767,8 +3139,14 @@
       <c r="F126" s="3" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G126" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="H126" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="6"/>
       <c r="B127" s="6"/>
       <c r="C127" s="6" t="s">
@@ -2783,8 +3161,10 @@
       <c r="F127" s="6" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G127" s="6"/>
+      <c r="H127" s="6"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="1"/>
       <c r="B128" s="1" t="s">
         <v>56</v>
@@ -2801,8 +3181,10 @@
       <c r="F128" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G128" s="1"/>
+      <c r="H128" s="1"/>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="6"/>
       <c r="B129" s="6"/>
       <c r="C129" s="6" t="s">
@@ -2817,8 +3199,10 @@
       <c r="F129" s="6" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G129" s="6"/>
+      <c r="H129" s="6"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="1"/>
       <c r="B130" s="1" t="s">
         <v>165</v>
@@ -2835,8 +3219,10 @@
       <c r="F130" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G130" s="1"/>
+      <c r="H130" s="1"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="6"/>
       <c r="B131" s="6" t="s">
         <v>153</v>
@@ -2853,6 +3239,8 @@
       <c r="F131" s="6" t="s">
         <v>74</v>
       </c>
+      <c r="G131" s="6"/>
+      <c r="H131" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
añado interfaces del backend
</commit_message>
<xml_diff>
--- a/Documentacion/Diccionario de datos.xlsx
+++ b/Documentacion/Diccionario de datos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="225">
   <si>
     <t>Tabla</t>
   </si>
@@ -1136,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G127" sqref="G127"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1950,7 +1950,9 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
-      <c r="B55" s="6"/>
+      <c r="B55" s="6" t="s">
+        <v>110</v>
+      </c>
       <c r="C55" s="6" t="s">
         <v>5</v>
       </c>

</xml_diff>